<commit_message>
conteo inicial + hojas de ruta
</commit_message>
<xml_diff>
--- a/Hojas de Ruta/Motores/Tambor Decanter/OT 26234 - BALANCEO TAMBOR DECANTER MS-936 .xlsx
+++ b/Hojas de Ruta/Motores/Tambor Decanter/OT 26234 - BALANCEO TAMBOR DECANTER MS-936 .xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmedina\Documents\GitHub\Repositorio-Git\MD-PlanificacionProduccion\Hojas de Ruta\Motores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmedina\Documents\GitHub\Repositorio-Git\MD-PlanificacionProduccion\Hojas de Ruta\Motores\Tambor Decanter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -95,10 +95,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H5"/>
+  <dimension ref="B1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:O1048576"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,12 +434,14 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G2" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="H2">
-        <v>0</v>
+      <c r="H2" s="4">
+        <v>0.26041666666666669</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -449,13 +457,13 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="G3" s="2">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -470,13 +478,13 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="G4" s="2">
         <v>0.25</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -491,15 +499,32 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G5" s="2">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="H5">
-        <v>0</v>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="2">
+        <f>SUM(F2:F5)</f>
+        <v>0.26041666666666669</v>
+      </c>
+      <c r="G6" s="2">
+        <f>SUM(G2:G5)</f>
+        <v>0.32291666666666663</v>
+      </c>
+      <c r="H6" s="2">
+        <f>SUM(H2:H5)</f>
+        <v>0.26041666666666669</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H2:H5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>